<commit_message>
update with old laptop
</commit_message>
<xml_diff>
--- a/stimuli/letter_width_TNR.xlsx
+++ b/stimuli/letter_width_TNR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\RS_dyslexia\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF15C8F1-CE4B-453A-8066-BC772120402F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E3F919-3DBA-4055-A425-31568C006CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A5B9554-20DA-4AB9-8169-E94E689EABD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>a</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>width</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -210,12 +213,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,9 +239,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -572,7 +584,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,8 +601,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -610,11 +625,11 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
-        <v>8</v>
+      <c r="B5" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -638,7 +653,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -654,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -662,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -670,7 +685,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -698,10 +713,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>4</v>
       </c>
     </row>
@@ -710,7 +725,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -718,7 +733,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -726,7 +741,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -734,7 +749,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -758,7 +773,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -766,7 +781,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -790,7 +805,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -823,6 +838,9 @@
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B32" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -862,7 +880,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -913,27 +931,33 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>